<commit_message>
Switched back to THVD2410
Decided that the cost / simplicity of just a THVD2410 was better
</commit_message>
<xml_diff>
--- a/Handheld DMX Console V3 DMX/Default Configuration/Outputs/BOM/BOM_PartType-Handheld DMX Console V3 DMX.xlsx
+++ b/Handheld DMX Console V3 DMX/Default Configuration/Outputs/BOM/BOM_PartType-Handheld DMX Console V3 DMX.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40A8D16B-BB2A-475B-8831-7CED739DE418}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F081FB0-91EC-464B-8A15-586D154E5DD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30405" yWindow="2130" windowWidth="21600" windowHeight="11385" xr2:uid="{0347B62B-CB02-4BEF-9589-A688766C52B0}"/>
+    <workbookView xWindow="30405" yWindow="2130" windowWidth="21600" windowHeight="11385" xr2:uid="{8B8686DC-20E5-4606-8E19-536479BCF211}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PartType-Handheld DMX Conso" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
   <si>
     <t>Comment</t>
   </si>
@@ -120,7 +120,7 @@
     <t>CMP-1012-00133-1</t>
   </si>
   <si>
-    <t>SN65HVD72DR</t>
+    <t>THVD2410</t>
   </si>
   <si>
     <t>3.3 V Supply RS-485 with IEC ESD Protection, 0.25 Mbps, -40 to 125 degC, 8-Pin SOIC, RoHS, Tape and Reel</t>
@@ -133,21 +133,6 @@
   </si>
   <si>
     <t>CMP-0694-00004-2</t>
-  </si>
-  <si>
-    <t>SM712.TCT</t>
-  </si>
-  <si>
-    <t>Asymmetrical TVS Diode for Extended Common-Mode RS-485, 400 W, -55 to 125 degC, 3-Pin SOT23, RoHS, Tape and Reel</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>SMTC-SOT23-3_V</t>
-  </si>
-  <si>
-    <t>CMP-2000-05357-1</t>
   </si>
   <si>
     <t>TPS76333DBVTG4</t>
@@ -569,8 +554,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E2DACC-36B3-43F9-A51B-D6BF68563497}">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E1E246-C203-45F1-B5BC-AB305F894E07}">
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -764,16 +749,16 @@
         <v>40</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F10" s="3">
         <v>1</v>
@@ -781,19 +766,19 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F11" s="3">
         <v>1</v>
@@ -801,41 +786,21 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F12" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>